<commit_message>
add attachment for csf
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/excelVendor.xlsx
+++ b/FMS.Website/files_upload/excelVendor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vox\task\fms021020170830\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vox\task\fms021020170830\hms-fms\FMS.Website\files_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>System</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>h44py</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <dimension ref="B2:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,8 +686,8 @@
       <c r="I4" s="3">
         <v>43099</v>
       </c>
-      <c r="J4" s="1" t="b">
-        <v>1</v>
+      <c r="J4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>34</v>
@@ -716,11 +722,11 @@
       <c r="U4" s="1">
         <v>1</v>
       </c>
-      <c r="V4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="W4" s="1" t="b">
-        <v>1</v>
+      <c r="V4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add mass upload from vendor in csf and temporary
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/excelVendor.xlsx
+++ b/FMS.Website/files_upload/excelVendor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>System</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Vat</t>
   </si>
   <si>
-    <t>Restituion</t>
-  </si>
-  <si>
     <t>gbf</t>
   </si>
   <si>
@@ -141,6 +138,15 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Surabaya</t>
+  </si>
+  <si>
+    <t>Restitution</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W5"/>
+  <dimension ref="B2:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,16 +558,17 @@
     <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -582,20 +589,21 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="4" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="6"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="6"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -639,46 +647,49 @@
       <c r="P3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="2" t="s">
-        <v>23</v>
+      <c r="X3" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3">
         <v>43065</v>
@@ -687,49 +698,52 @@
         <v>43099</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="M4" s="1">
         <v>2016</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>2017</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1</v>
       </c>
       <c r="U4" s="1">
         <v>1</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -752,13 +766,14 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:J2"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="K2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>